<commit_message>
modify dea input sample, finish all features
</commit_message>
<xml_diff>
--- a/input/DEA_input_dataset.xlsx
+++ b/input/DEA_input_dataset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Bus Line</t>
   </si>
@@ -34,6 +34,63 @@
   </si>
   <si>
     <t>Customer</t>
+  </si>
+  <si>
+    <t>2X</t>
+  </si>
+  <si>
+    <t>F590</t>
+  </si>
+  <si>
+    <t>F518</t>
+  </si>
+  <si>
+    <t>F514</t>
+  </si>
+  <si>
+    <t>F618</t>
+  </si>
+  <si>
+    <t>F504</t>
+  </si>
+  <si>
+    <t>F534</t>
+  </si>
+  <si>
+    <t>F638</t>
+  </si>
+  <si>
+    <t>F522</t>
+  </si>
+  <si>
+    <t>F400</t>
+  </si>
+  <si>
+    <t>F402</t>
+  </si>
+  <si>
+    <t>F94</t>
+  </si>
+  <si>
+    <t>F556</t>
+  </si>
+  <si>
+    <t>F570</t>
+  </si>
+  <si>
+    <t>F547</t>
+  </si>
+  <si>
+    <t>F546</t>
+  </si>
+  <si>
+    <t>F401</t>
+  </si>
+  <si>
+    <t>F578</t>
+  </si>
+  <si>
+    <t>35M</t>
   </si>
 </sst>
 </file>
@@ -858,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2481,6 +2538,431 @@
         <v>192.09128128500001</v>
       </c>
     </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>450.14666666699998</v>
+      </c>
+      <c r="C96">
+        <v>772.99052977199995</v>
+      </c>
+      <c r="D96">
+        <v>12</v>
+      </c>
+      <c r="E96">
+        <v>19.091281285000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97">
+        <v>269.36</v>
+      </c>
+      <c r="C97">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D97">
+        <v>4</v>
+      </c>
+      <c r="E97">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98">
+        <v>269.36</v>
+      </c>
+      <c r="C98">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D98">
+        <v>4</v>
+      </c>
+      <c r="E98">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99">
+        <v>269.36</v>
+      </c>
+      <c r="C99">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D99">
+        <v>4</v>
+      </c>
+      <c r="E99">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>9</v>
+      </c>
+      <c r="B100">
+        <v>269.36</v>
+      </c>
+      <c r="C100">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D100">
+        <v>4</v>
+      </c>
+      <c r="E100">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101">
+        <v>269.36</v>
+      </c>
+      <c r="C101">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D101">
+        <v>4</v>
+      </c>
+      <c r="E101">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102">
+        <v>269.36</v>
+      </c>
+      <c r="C102">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D102">
+        <v>4</v>
+      </c>
+      <c r="E102">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103">
+        <v>269.36</v>
+      </c>
+      <c r="C103">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D103">
+        <v>4</v>
+      </c>
+      <c r="E103">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104">
+        <v>269.36</v>
+      </c>
+      <c r="C104">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D104">
+        <v>4</v>
+      </c>
+      <c r="E104">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105">
+        <v>269.36</v>
+      </c>
+      <c r="C105">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D105">
+        <v>4</v>
+      </c>
+      <c r="E105">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>15</v>
+      </c>
+      <c r="B106">
+        <v>269.36</v>
+      </c>
+      <c r="C106">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D106">
+        <v>4</v>
+      </c>
+      <c r="E106">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>16</v>
+      </c>
+      <c r="B107">
+        <v>269.36</v>
+      </c>
+      <c r="C107">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D107">
+        <v>4</v>
+      </c>
+      <c r="E107">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>17</v>
+      </c>
+      <c r="B108">
+        <v>269.36</v>
+      </c>
+      <c r="C108">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D108">
+        <v>4</v>
+      </c>
+      <c r="E108">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109">
+        <v>269.36</v>
+      </c>
+      <c r="C109">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D109">
+        <v>4</v>
+      </c>
+      <c r="E109">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>19</v>
+      </c>
+      <c r="B110">
+        <v>269.36</v>
+      </c>
+      <c r="C110">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D110">
+        <v>4</v>
+      </c>
+      <c r="E110">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>20</v>
+      </c>
+      <c r="B111">
+        <v>269.36</v>
+      </c>
+      <c r="C111">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D111">
+        <v>4</v>
+      </c>
+      <c r="E111">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112">
+        <v>269.36</v>
+      </c>
+      <c r="C112">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D112">
+        <v>4</v>
+      </c>
+      <c r="E112">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>22</v>
+      </c>
+      <c r="B113">
+        <v>269.36</v>
+      </c>
+      <c r="C113">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D113">
+        <v>4</v>
+      </c>
+      <c r="E113">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114">
+        <v>701</v>
+      </c>
+      <c r="B114">
+        <v>269.36</v>
+      </c>
+      <c r="C114">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D114">
+        <v>4</v>
+      </c>
+      <c r="E114">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115">
+        <v>703</v>
+      </c>
+      <c r="B115">
+        <v>269.36</v>
+      </c>
+      <c r="C115">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D115">
+        <v>4</v>
+      </c>
+      <c r="E115">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116">
+        <v>628</v>
+      </c>
+      <c r="B116">
+        <v>269.36</v>
+      </c>
+      <c r="C116">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D116">
+        <v>4</v>
+      </c>
+      <c r="E116">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117">
+        <v>704</v>
+      </c>
+      <c r="B117">
+        <v>269.36</v>
+      </c>
+      <c r="C117">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D117">
+        <v>4</v>
+      </c>
+      <c r="E117">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118">
+        <v>750</v>
+      </c>
+      <c r="B118">
+        <v>269.36</v>
+      </c>
+      <c r="C118">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D118">
+        <v>4</v>
+      </c>
+      <c r="E118">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119">
+        <v>720</v>
+      </c>
+      <c r="B119">
+        <v>269.36</v>
+      </c>
+      <c r="C119">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D119">
+        <v>4</v>
+      </c>
+      <c r="E119">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120">
+        <v>269.36</v>
+      </c>
+      <c r="C120">
+        <v>400.12379214399999</v>
+      </c>
+      <c r="D120">
+        <v>4</v>
+      </c>
+      <c r="E120">
+        <v>101.52455476199999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>